<commit_message>
schema: spreadsheets: 2 minor changes
Update to latest version of standard

Set ENUM for source type.

Remove 2 options from a project field.
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/organisation_public_v003.xlsx
+++ b/indigo/spreadsheetform_guides/organisation_public_v003.xlsx
@@ -1569,7 +1569,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2185,7 +2185,7 @@
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" customFormat="false" ht="115.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="32" t="s">
         <v>73</v>
       </c>
@@ -2533,7 +2533,7 @@
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C11:C39" type="list">
-      <formula1>"Contract,Report,Award notice,Website"</formula1>
+      <formula1>"Contract,Report,Award Notice,Website,News piece,Press release,Email correspondence,Evaluation report"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>